<commit_message>
add explanatory text file
</commit_message>
<xml_diff>
--- a/003.xlsx
+++ b/003.xlsx
@@ -4823,7 +4823,7 @@
     <t>North Macedonia</t>
   </si>
   <si>
-    <t>Republic Of Moldova</t>
+    <t>Moldova</t>
   </si>
   <si>
     <t>Russian Federation</t>
@@ -4862,7 +4862,7 @@
     <t>Bermuda</t>
   </si>
   <si>
-    <t>Bolivia (Plurinational State Of)</t>
+    <t>Bolivia</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -4925,7 +4925,7 @@
     <t>Uruguay</t>
   </si>
   <si>
-    <t>Venezuela (Bolivarian Republic Of)</t>
+    <t>Venezuela</t>
   </si>
   <si>
     <t>Afghanistan</t>
@@ -4952,7 +4952,7 @@
     <t>Guam</t>
   </si>
   <si>
-    <t>China, Hong Kong Special Administrative Region</t>
+    <t>Hong Kong</t>
   </si>
   <si>
     <t>India</t>
@@ -4961,7 +4961,7 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Iran (Islamic Republic Of)</t>
+    <t>Iran</t>
   </si>
   <si>
     <t>Iraq</t>

</xml_diff>